<commit_message>
updated some reference files and added mining to IPPU production. Next step is to add wood to INEN
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_af_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_af_calibrated.xlsx
@@ -82597,112 +82597,112 @@
         <v>0.5158371040723981</v>
       </c>
       <c r="J655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS655">
-        <v>49.3298401180542</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="656" spans="1:45">
@@ -82725,112 +82725,112 @@
         <v>0.1661392405063291</v>
       </c>
       <c r="J656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS656">
-        <v>73.3539640322938</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="657" spans="1:45">
@@ -82853,112 +82853,112 @@
         <v>0.2412868632707775</v>
       </c>
       <c r="J657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS657">
-        <v>14.8797908834307</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="658" spans="1:45">
@@ -82981,112 +82981,112 @@
         <v>0.2842377260981913</v>
       </c>
       <c r="J658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS658">
-        <v>62.0714569028575</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="659" spans="1:45">
@@ -83109,112 +83109,112 @@
         <v>0.5276595744680851</v>
       </c>
       <c r="J659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS659">
-        <v>88.73803640142491</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="660" spans="1:45">
@@ -83237,112 +83237,112 @@
         <v>0.5276595744680851</v>
       </c>
       <c r="J660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS660">
-        <v>43.7103746958584</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="661" spans="1:45">
@@ -83365,112 +83365,112 @@
         <v>0.4508580343213729</v>
       </c>
       <c r="J661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="K661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="L661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="M661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="N661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="O661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="P661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Q661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="R661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="S661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="T661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="U661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="V661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="W661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="X661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Y661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="Z661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AA661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AB661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AC661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AD661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AE661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AF661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AG661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AH661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AI661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AJ661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AK661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AL661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AM661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AN661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AO661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AP661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AQ661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AR661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
       <c r="AS661">
-        <v>33.8203147315285</v>
+        <v>42.86511000455413</v>
       </c>
     </row>
     <row r="662" spans="1:45">

</xml_diff>